<commit_message>
My Store first commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{14C975A1-CF5F-4617-9617-7D3715E57EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1E49349E-AD49-4CB9-BF4F-8D663A066ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O16"/>
+  <oleSize ref="A1:L16"/>
 </workbook>
 </file>
 
@@ -730,23 +730,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="4" width="26.21875" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="44.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="10" max="10" width="23.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" customWidth="1"/>
+    <col min="13" max="13" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -762,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>43</v>
       </c>
@@ -770,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>38</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -796,7 +796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -813,7 +813,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -830,7 +830,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -847,7 +847,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -864,7 +864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -881,7 +881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -929,7 +929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -990,16 +990,16 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>50</v>
       </c>
@@ -1031,17 +1031,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>58</v>
       </c>
@@ -1063,9 +1063,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -1098,14 +1098,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -1123,19 +1123,19 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>52</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>76</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>77</v>
       </c>

</xml_diff>